<commit_message>
Updating llm_agents to run on azure vm better
</commit_message>
<xml_diff>
--- a/VMs.xlsx
+++ b/VMs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aayus\OneDrive\Desktop\AI workspace\Vulnerabilities\vm-command-runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F2656A-DCA6-48DF-A9AF-794D580738B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008B46E2-66C1-482E-AF60-3277FC4B6C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,13 +31,13 @@
     <t>Command</t>
   </si>
   <si>
-    <t>vm-test-1</t>
-  </si>
-  <si>
     <t>vm-rg-1</t>
   </si>
   <si>
     <t>pwd</t>
+  </si>
+  <si>
+    <t>vm-openssl-test</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,13 +426,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting error in excel file
</commit_message>
<xml_diff>
--- a/VMs.xlsx
+++ b/VMs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aayus\OneDrive\Desktop\AI workspace\Vulnerabilities\vm-llm-runner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aayus\OneDrive\Desktop\AI workspace\Vulnerabilities\vm-command-runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE28E10E-DD56-4DB9-ACE9-D711CD3FF144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478707A8-C434-4618-B646-73134ED63269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>solution_summary</t>
   </si>
   <si>
-    <t>lop-test</t>
-  </si>
-  <si>
     <t>pwd</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>Update "OpenSSL" to version 1.1.1n or later</t>
+  </si>
+  <si>
+    <t>log-test</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,22 +493,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code update from Dharmik
</commit_message>
<xml_diff>
--- a/VMs.xlsx
+++ b/VMs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aayus\OneDrive\Desktop\AI workspace\Vulnerabilities\vm-command-runner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aayush.Tomar\Code workspace\Vulnerabilities\vm-command-runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478707A8-C434-4618-B646-73134ED63269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14AEEE7-063A-4D25-9E6C-8485080ADF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,25 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Ubuntu</t>
-  </si>
-  <si>
-    <t>3.1.1</t>
-  </si>
-  <si>
-    <t>vm_name</t>
-  </si>
-  <si>
-    <t>os_type</t>
-  </si>
-  <si>
-    <t>command</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>cve</t>
   </si>
@@ -46,9 +28,6 @@
     <t>solution_summary</t>
   </si>
   <si>
-    <t>pwd</t>
-  </si>
-  <si>
     <t>CVE-2022-0778</t>
   </si>
   <si>
@@ -56,13 +35,52 @@
   </si>
   <si>
     <t>log-test</t>
+  </si>
+  <si>
+    <t>Cloud Account/Subscription Name</t>
+  </si>
+  <si>
+    <t>VM Name</t>
+  </si>
+  <si>
+    <t>commands</t>
+  </si>
+  <si>
+    <t>Azure subscription 1</t>
+  </si>
+  <si>
+    <t>window-vm-test</t>
+  </si>
+  <si>
+    <t>echo "Updating openssl to version 1.1.1n"
+echo "failed to update openssl to version 1.1.1n" &gt;&amp;2</t>
+  </si>
+  <si>
+    <t>echo "Updating Windows to version 20H2"
+echo "failed to update Windows to version 20H2" &gt;&amp;2</t>
+  </si>
+  <si>
+    <t>CVE-2021-34527</t>
+  </si>
+  <si>
+    <t>Update "Windows" to version 20H2 or later</t>
+  </si>
+  <si>
+    <t>echo "Updating Linux Kernel to version 5.4.0"
+echo "failed to update Linux Kernel to version 5.4.0" &gt;&amp;2</t>
+  </si>
+  <si>
+    <t>CVE-2021-22918</t>
+  </si>
+  <si>
+    <t>Update "Linux Kernel" to version 5.4.0 or later</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,12 +98,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFDCDCAA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FF569CD6"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="8"/>
       <color rgb="FFDCDCAA"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -99,27 +136,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -137,18 +159,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -455,63 +486,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="41.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d0cb1e24-a0e2-4a4c-9340-733297c9cd7c}" enabled="1" method="Privileged" siteId="{db1e96a8-a3da-442a-930b-235cac24cd5c}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Fixing the Windows vm name in the excel file
</commit_message>
<xml_diff>
--- a/VMs.xlsx
+++ b/VMs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aayush.Tomar\Code workspace\Vulnerabilities\vm-command-runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14AEEE7-063A-4D25-9E6C-8485080ADF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5724D2D7-A86F-4D66-A142-CC14D058F5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>Azure subscription 1</t>
   </si>
   <si>
-    <t>window-vm-test</t>
-  </si>
-  <si>
     <t>echo "Updating openssl to version 1.1.1n"
 echo "failed to update openssl to version 1.1.1n" &gt;&amp;2</t>
   </si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>Update "Linux Kernel" to version 5.4.0 or later</t>
+  </si>
+  <si>
+    <t>windows-vm-test</t>
   </si>
 </sst>
 </file>
@@ -489,20 +489,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -520,7 +520,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -528,7 +528,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>2</v>
@@ -538,7 +538,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -546,16 +546,16 @@
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -563,30 +563,30 @@
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="5" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating excel file for demo
</commit_message>
<xml_diff>
--- a/VMs.xlsx
+++ b/VMs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aayush.Tomar\Code workspace\Vulnerabilities\vm-command-runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1F6D2F-EDF9-4EFC-A4D8-97B71A578120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F831B9DA-0F46-4F58-B11A-EFD6702CA526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>cve</t>
   </si>
@@ -40,7 +40,13 @@
     <t>AZ-AS-SUB-EX-N-SEQ02125-CORE</t>
   </si>
   <si>
-    <t>windows-script1</t>
+    <t>CVE-Shell-Test-Windows</t>
+  </si>
+  <si>
+    <t>update python version to 3.11.9</t>
+  </si>
+  <si>
+    <t>windows-demo</t>
   </si>
   <si>
     <t># Define version and download path
@@ -50,15 +56,24 @@
 # Download the installer
 Invoke-WebRequest -Uri $installerUrl -OutFile $installerPath -UseBasicParsing
 # Run the installer silently
-Start-Process -FilePath $installerPath -ArgumentList "/quiet InstallAllUsers=1 PrependPath=1 Include_test=0" -Wait
-# Optional: Verify installation
-python --version</t>
-  </si>
-  <si>
-    <t>CVE-Shell-Test-Windows</t>
-  </si>
-  <si>
-    <t>update python version to 3.11.9</t>
+Start-Process -FilePath $installerPath -ArgumentList "/quiet InstallAllUsers=1 PrependPath=1 Include_test=0" -Wait</t>
+  </si>
+  <si>
+    <t>linux-demo</t>
+  </si>
+  <si>
+    <t># Update package lists
+sudo apt update
+# Install a specific version of openssl (3.0.14)
+sudo apt install openssl=3.0.14-1~$(lsb_release -cs)1
+# Hold the package at this version (optional)
+sudo apt-mark hold openssl</t>
+  </si>
+  <si>
+    <t>CVE-Shell-Test-Ubuntu</t>
+  </si>
+  <si>
+    <t>Update openssl version to 3.0.14</t>
   </si>
 </sst>
 </file>
@@ -474,7 +489,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,29 +520,40 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>

</xml_diff>

<commit_message>
Final excel update for demo
</commit_message>
<xml_diff>
--- a/VMs.xlsx
+++ b/VMs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aayush.Tomar\Code workspace\Vulnerabilities\vm-command-runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F831B9DA-0F46-4F58-B11A-EFD6702CA526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A74DEEA-1A69-4E11-B4EA-D886C0168D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,23 @@
     <t>windows-demo</t>
   </si>
   <si>
+    <t>linux-demo</t>
+  </si>
+  <si>
+    <t># Update package lists
+sudo apt update
+# Install a specific version of openssl (3.0.14)
+sudo apt install openssl=3.0.14-1~$(lsb_release -cs)1
+# Hold the package at this version (optional)
+sudo apt-mark hold openssl</t>
+  </si>
+  <si>
+    <t>CVE-Shell-Test-Ubuntu</t>
+  </si>
+  <si>
+    <t>Update openssl version to 3.0.14</t>
+  </si>
+  <si>
     <t># Define version and download path
 $pythonVersion = "3.11.9"
 $installerUrl = "https://www.python.org/ftp/python/$pythonVersion/python-$pythonVersion-amd64.exe"
@@ -56,24 +73,9 @@
 # Download the installer
 Invoke-WebRequest -Uri $installerUrl -OutFile $installerPath -UseBasicParsing
 # Run the installer silently
-Start-Process -FilePath $installerPath -ArgumentList "/quiet InstallAllUsers=1 PrependPath=1 Include_test=0" -Wait</t>
-  </si>
-  <si>
-    <t>linux-demo</t>
-  </si>
-  <si>
-    <t># Update package lists
-sudo apt update
-# Install a specific version of openssl (3.0.14)
-sudo apt install openssl=3.0.14-1~$(lsb_release -cs)1
-# Hold the package at this version (optional)
-sudo apt-mark hold openssl</t>
-  </si>
-  <si>
-    <t>CVE-Shell-Test-Ubuntu</t>
-  </si>
-  <si>
-    <t>Update openssl version to 3.0.14</t>
+Start-Process -FilePath $installerPath -ArgumentList "/quiet InstallAllUsers=1 PrependPath=1 Include_test=0" -Wait
+$env:Path = [System.Environment]::GetEnvironmentVariable("Path", [System.EnvironmentVariableTarget]::Machine)
+python --version</t>
   </si>
 </sst>
 </file>
@@ -489,20 +491,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -520,7 +522,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -528,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>6</v>
@@ -538,30 +540,30 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>

</xml_diff>